<commit_message>
Rebalancing to excel file, not filling in between dates
</commit_message>
<xml_diff>
--- a/data/output.xlsx
+++ b/data/output.xlsx
@@ -446,3841 +446,3841 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-04-30</t>
+          <t>2024-04-01</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.05402733015411746</v>
+        <v>-0.09857054487816309</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.06364370641325599</v>
+        <v>-0.1150990622218154</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.02000319774194514</v>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-05-30</t>
+          <t>2024-05-01</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.05402733015411746</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.06364370641325599</v>
+        <v>-0.1150990622218154</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.03787151907763749</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-06-30</t>
+          <t>2024-06-01</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.05402733015411746</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.1150990622218154</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.02000319774194514</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-07-30</t>
+          <t>2024-07-01</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.02000319774194514</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-08-30</t>
+          <t>2024-08-01</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C6" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.01005962170770122</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-09-30</t>
+          <t>2024-09-01</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0001160456734573077</v>
+        <v/>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-10-30</t>
+          <t>2024-10-01</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C8" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0001160456734573077</v>
+        <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-11-30</t>
+          <t>2024-11-01</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C9" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D9" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-12-30</t>
+          <t>2024-12-01</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C10" t="n">
-        <v>0.07952873638064348</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D10" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-01-30</t>
+          <t>2025-01-01</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C11" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.01005962170770122</v>
+        <v/>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-02-28</t>
+          <t>2025-02-01</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.03787151907763749</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2025-03-01</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C13" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D13" t="n">
-        <v>0.02971468242927444</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-04-30</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.06991236012150494</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C14" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D14" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-05-30</t>
+          <t>2025-05-01</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.06991236012150494</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C15" t="n">
-        <v>0.07952873638064348</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.0001160456734573077</v>
+        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-06-30</t>
+          <t>2025-06-01</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.06991236012150494</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C16" t="n">
-        <v>0.07952873638064348</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D16" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-07-30</t>
+          <t>2025-07-01</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.06991236012150494</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C17" t="n">
-        <v>0.07952873638064348</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-08-30</t>
+          <t>2025-08-01</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.06991236012150494</v>
+        <v>-0.09857054487816309</v>
       </c>
       <c r="C18" t="n">
-        <v>0.07952873638064348</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D18" t="n">
-        <v>0.02971468242927444</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-09-30</t>
+          <t>2025-09-01</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.06991236012150494</v>
+        <v>-0.09857054487816309</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1081632249394234</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D19" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-10-01</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.06991236012150494</v>
+        <v>-0.09857054487816309</v>
       </c>
       <c r="C20" t="n">
-        <v>0.1081632249394234</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D20" t="n">
-        <v>0.02971468242927444</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-11-30</t>
+          <t>2025-11-01</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.09470029817662944</v>
+        <v>-0.09857054487816309</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1081632249394234</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D21" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-12-30</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.05402733015411746</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.06364370641325599</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2026-01-30</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.05402733015411746</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.06364370641325599</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2026-02-28</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.05402733015411746</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2026-03-30</t>
+          <t>2026-03-01</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.05402733015411746</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2026-04-30</t>
+          <t>2026-04-01</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.06364370641325599</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.02994677377618906</v>
+        <v>-0.03787151907763749</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2026-05-30</t>
+          <t>2026-05-01</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.06364370641325599</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.02994677377618906</v>
+        <v>-0.03787151907763749</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2026-06-30</t>
+          <t>2026-06-01</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.06364370641325599</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.01005962170770122</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-07-30</t>
+          <t>2026-07-01</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C29" t="n">
-        <v>-0.06364370641325599</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.01005962170770122</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2026-08-30</t>
+          <t>2026-08-01</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C30" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.02000319774194514</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2026-09-30</t>
+          <t>2026-09-01</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.02000319774194514</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2026-10-30</t>
+          <t>2026-10-01</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C32" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D32" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2026-11-30</t>
+          <t>2026-11-01</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D33" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2026-12-30</t>
+          <t>2026-12-01</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.02000319774194514</v>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2027-01-30</t>
+          <t>2027-01-01</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.02000319774194514</v>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2027-02-28</t>
+          <t>2027-02-01</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C36" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.02000319774194514</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2027-03-30</t>
+          <t>2027-03-01</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C37" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.02000319774194514</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2027-04-30</t>
+          <t>2027-04-01</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C38" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D38" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2027-05-30</t>
+          <t>2027-05-01</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C39" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D39" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2027-06-30</t>
+          <t>2027-06-01</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C40" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.02000319774194514</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2027-07-30</t>
+          <t>2027-07-01</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C41" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.02000319774194514</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2027-08-30</t>
+          <t>2027-08-01</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.09857054487816309</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.1150990622218154</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2027-09-30</t>
+          <t>2027-09-01</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.09857054487816309</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.1150990622218154</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2027-10-30</t>
+          <t>2027-10-01</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.09857054487816309</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.1150990622218154</v>
       </c>
       <c r="D44" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2027-11-30</t>
+          <t>2027-11-01</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.1150990622218154</v>
       </c>
       <c r="D45" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2027-12-30</t>
+          <t>2027-12-01</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C46" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.1150990622218154</v>
       </c>
       <c r="D46" t="n">
-        <v>0.02971468242927444</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2028-01-30</t>
+          <t>2028-01-01</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C47" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.1150990622218154</v>
       </c>
       <c r="D47" t="n">
-        <v>0.02971468242927444</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2028-02-29</t>
+          <t>2028-02-01</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C48" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2028-03-30</t>
+          <t>2028-03-01</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C49" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2028-04-30</t>
+          <t>2028-04-01</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C50" t="n">
-        <v>0.07952873638064348</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D50" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2028-05-30</t>
+          <t>2028-05-01</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C51" t="n">
-        <v>0.07952873638064348</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D51" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2028-06-30</t>
+          <t>2028-06-01</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C52" t="n">
-        <v>0.07952873638064348</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D52" t="n">
-        <v>0.02971468242927444</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2028-07-30</t>
+          <t>2028-07-01</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C53" t="n">
-        <v>0.07952873638064348</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D53" t="n">
-        <v>0.02971468242927444</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2028-08-30</t>
+          <t>2028-08-01</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.03787151907763749</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2028-09-30</t>
+          <t>2028-09-01</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.03787151907763749</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2028-10-30</t>
+          <t>2028-10-01</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D56" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.03787151907763749</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2028-11-30</t>
+          <t>2028-11-01</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C57" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D57" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2028-12-30</t>
+          <t>2028-12-01</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C58" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D58" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2029-01-30</t>
+          <t>2029-01-01</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C59" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D59" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2029-02-28</t>
+          <t>2029-02-01</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C60" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D60" t="n">
-        <v>-0.02000319774194514</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2029-03-30</t>
+          <t>2029-03-01</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C61" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D61" t="n">
-        <v>-0.02000319774194514</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2029-04-30</t>
+          <t>2029-04-01</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C62" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D62" t="n">
-        <v>-0.02000319774194514</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2029-05-30</t>
+          <t>2029-05-01</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C63" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D63" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2029-06-30</t>
+          <t>2029-06-01</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C64" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D64" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2029-07-30</t>
+          <t>2029-07-01</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C65" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D65" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2029-08-30</t>
+          <t>2029-08-01</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C66" t="n">
-        <v>0.07952873638064348</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D66" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2029-09-30</t>
+          <t>2029-09-01</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C67" t="n">
-        <v>0.07952873638064348</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D67" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2029-10-30</t>
+          <t>2029-10-01</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C68" t="n">
-        <v>0.07952873638064348</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D68" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2029-11-30</t>
+          <t>2029-11-01</t>
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.06991236012150494</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C69" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D69" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2029-12-30</t>
+          <t>2029-12-01</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.06991236012150494</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C70" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D70" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2030-01-30</t>
+          <t>2030-01-01</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>0.06991236012150494</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C71" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D71" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2030-02-28</t>
+          <t>2030-02-01</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D72" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2030-03-30</t>
+          <t>2030-03-01</t>
         </is>
       </c>
       <c r="B73" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C73" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D73" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2030-04-30</t>
+          <t>2030-04-01</t>
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D74" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2030-05-30</t>
+          <t>2030-05-01</t>
         </is>
       </c>
       <c r="B75" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C75" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D75" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2030-06-30</t>
+          <t>2030-06-01</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C76" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D76" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2030-07-30</t>
+          <t>2030-07-01</t>
         </is>
       </c>
       <c r="B77" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C77" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D77" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2030-08-30</t>
+          <t>2030-08-01</t>
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C78" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D78" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2030-09-30</t>
+          <t>2030-09-01</t>
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C79" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D79" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2030-10-30</t>
+          <t>2030-10-01</t>
         </is>
       </c>
       <c r="B80" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C80" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D80" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2030-11-30</t>
+          <t>2030-11-01</t>
         </is>
       </c>
       <c r="B81" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C81" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D81" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2030-12-30</t>
+          <t>2030-12-01</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C82" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D82" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2031-01-30</t>
+          <t>2031-01-01</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C83" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D83" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2031-02-28</t>
+          <t>2031-02-01</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C84" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D84" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2031-03-30</t>
+          <t>2031-03-01</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C85" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D85" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2031-04-30</t>
+          <t>2031-04-01</t>
         </is>
       </c>
       <c r="B86" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C86" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D86" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2031-05-30</t>
+          <t>2031-05-01</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C87" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D87" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2031-06-30</t>
+          <t>2031-06-01</t>
         </is>
       </c>
       <c r="B88" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C88" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D88" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2031-07-30</t>
+          <t>2031-07-01</t>
         </is>
       </c>
       <c r="B89" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C89" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D89" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2031-08-30</t>
+          <t>2031-08-01</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C90" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D90" t="n">
-        <v>-0.01005962170770122</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2031-09-30</t>
+          <t>2031-09-01</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C91" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D91" t="n">
-        <v>-0.01005962170770122</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2031-10-30</t>
+          <t>2031-10-01</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C92" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D92" t="n">
-        <v>-0.01005962170770122</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2031-11-30</t>
+          <t>2031-11-01</t>
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C93" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D93" t="n">
-        <v>-0.01005962170770122</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2031-12-30</t>
+          <t>2031-12-01</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C94" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D94" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2032-01-30</t>
+          <t>2032-01-01</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C95" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D95" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2032-02-29</t>
+          <t>2032-02-01</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C96" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D96" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2032-03-30</t>
+          <t>2032-03-01</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C97" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D97" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2032-04-30</t>
+          <t>2032-04-01</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C98" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D98" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2032-05-30</t>
+          <t>2032-05-01</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C99" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D99" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2032-06-30</t>
+          <t>2032-06-01</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C100" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D100" t="n">
-        <v>0.01977110639503053</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2032-07-30</t>
+          <t>2032-07-01</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C101" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D101" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2032-08-30</t>
+          <t>2032-08-01</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C102" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D102" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2032-09-30</t>
+          <t>2032-09-01</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C103" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D103" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2032-10-30</t>
+          <t>2032-10-01</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C104" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D104" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2032-11-30</t>
+          <t>2032-11-01</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C105" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D105" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2032-12-30</t>
+          <t>2032-12-01</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C106" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D106" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2033-01-30</t>
+          <t>2033-01-01</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C107" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D107" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2033-02-28</t>
+          <t>2033-02-01</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C108" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D108" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2033-03-30</t>
+          <t>2033-03-01</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C109" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D109" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2033-04-30</t>
+          <t>2033-04-01</t>
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C110" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D110" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2033-05-30</t>
+          <t>2033-05-01</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C111" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D111" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2033-06-30</t>
+          <t>2033-06-01</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C112" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D112" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2033-07-30</t>
+          <t>2033-07-01</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C113" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D113" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2033-08-30</t>
+          <t>2033-08-01</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C114" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D114" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2033-09-30</t>
+          <t>2033-09-01</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C115" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D115" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2033-10-30</t>
+          <t>2033-10-01</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C116" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D116" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2033-11-30</t>
+          <t>2033-11-01</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C117" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D117" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2033-12-30</t>
+          <t>2033-12-01</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C118" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D118" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2034-01-30</t>
+          <t>2034-01-01</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C119" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D119" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2034-02-28</t>
+          <t>2034-02-01</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C120" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D120" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2034-03-30</t>
+          <t>2034-03-01</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C121" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D121" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2034-04-30</t>
+          <t>2034-04-01</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C122" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D122" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2034-05-30</t>
+          <t>2034-05-01</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C123" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D123" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2034-06-30</t>
+          <t>2034-06-01</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C124" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D124" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2034-07-30</t>
+          <t>2034-07-01</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C125" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D125" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2034-08-30</t>
+          <t>2034-08-01</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C126" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D126" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2034-09-30</t>
+          <t>2034-09-01</t>
         </is>
       </c>
       <c r="B127" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C127" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D127" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2034-10-30</t>
+          <t>2034-10-01</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C128" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D128" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2034-11-30</t>
+          <t>2034-11-01</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C129" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D129" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2034-12-30</t>
+          <t>2034-12-01</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C130" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D130" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2035-01-30</t>
+          <t>2035-01-01</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C131" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D131" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2035-02-28</t>
+          <t>2035-02-01</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C132" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D132" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2035-03-30</t>
+          <t>2035-03-01</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C133" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D133" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2035-04-30</t>
+          <t>2035-04-01</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C134" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D134" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2035-05-30</t>
+          <t>2035-05-01</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C135" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D135" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2035-06-30</t>
+          <t>2035-06-01</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C136" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D136" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2035-07-30</t>
+          <t>2035-07-01</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C137" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D137" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2035-08-30</t>
+          <t>2035-08-01</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C138" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D138" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2035-09-30</t>
+          <t>2035-09-01</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C139" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D139" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2035-10-30</t>
+          <t>2035-10-01</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C140" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D140" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2035-11-30</t>
+          <t>2035-11-01</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C141" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D141" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2035-12-30</t>
+          <t>2035-12-01</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C142" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D142" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2036-01-30</t>
+          <t>2036-01-01</t>
         </is>
       </c>
       <c r="B143" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C143" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D143" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2036-02-29</t>
+          <t>2036-02-01</t>
         </is>
       </c>
       <c r="B144" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C144" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D144" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2036-03-30</t>
+          <t>2036-03-01</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C145" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D145" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2036-04-30</t>
+          <t>2036-04-01</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C146" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D146" t="n">
-        <v>-0.01005962170770122</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2036-05-30</t>
+          <t>2036-05-01</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C147" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D147" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2036-06-30</t>
+          <t>2036-06-01</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C148" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D148" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2036-07-30</t>
+          <t>2036-07-01</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C149" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D149" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2036-08-30</t>
+          <t>2036-08-01</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C150" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D150" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2036-09-30</t>
+          <t>2036-09-01</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C151" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D151" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2036-10-30</t>
+          <t>2036-10-01</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C152" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D152" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2036-11-30</t>
+          <t>2036-11-01</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C153" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D153" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2036-12-30</t>
+          <t>2036-12-01</t>
         </is>
       </c>
       <c r="B154" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C154" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D154" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2037-01-30</t>
+          <t>2037-01-01</t>
         </is>
       </c>
       <c r="B155" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C155" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D155" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2037-02-28</t>
+          <t>2037-02-01</t>
         </is>
       </c>
       <c r="B156" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C156" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D156" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2037-03-30</t>
+          <t>2037-03-01</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C157" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D157" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2037-04-30</t>
+          <t>2037-04-01</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C158" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D158" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2037-05-30</t>
+          <t>2037-05-01</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C159" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D159" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2037-06-30</t>
+          <t>2037-06-01</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C160" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D160" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2037-07-30</t>
+          <t>2037-07-01</t>
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C161" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D161" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2037-08-30</t>
+          <t>2037-08-01</t>
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C162" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D162" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2037-09-30</t>
+          <t>2037-09-01</t>
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C163" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D163" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2037-10-30</t>
+          <t>2037-10-01</t>
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C164" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D164" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2037-11-30</t>
+          <t>2037-11-01</t>
         </is>
       </c>
       <c r="B165" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C165" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D165" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2037-12-30</t>
+          <t>2037-12-01</t>
         </is>
       </c>
       <c r="B166" t="n">
-        <v>0.02033648401125598</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C166" t="n">
-        <v>0.02225975926308368</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D166" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2038-01-30</t>
+          <t>2038-01-01</t>
         </is>
       </c>
       <c r="B167" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C167" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D167" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2038-02-28</t>
+          <t>2038-02-01</t>
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C168" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D168" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2038-03-30</t>
+          <t>2038-03-01</t>
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C169" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D169" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2038-04-30</t>
+          <t>2038-04-01</t>
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C170" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D170" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2038-05-30</t>
+          <t>2038-05-01</t>
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C171" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D171" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2038-06-30</t>
+          <t>2038-06-01</t>
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C172" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D172" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>2038-07-30</t>
+          <t>2038-07-01</t>
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C173" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D173" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>2038-08-30</t>
+          <t>2038-08-01</t>
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.04512442206638047</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C174" t="n">
-        <v>0.05089424782186359</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D174" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>2038-09-30</t>
+          <t>2038-09-01</t>
         </is>
       </c>
       <c r="B175" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C175" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D175" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>2038-10-30</t>
+          <t>2038-10-01</t>
         </is>
       </c>
       <c r="B176" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C176" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D176" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>2038-11-30</t>
+          <t>2038-11-01</t>
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0.04512442206638047</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C177" t="n">
-        <v>0.05089424782186359</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D177" t="n">
-        <v>0.01977110639503053</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>2038-12-30</t>
+          <t>2038-12-01</t>
         </is>
       </c>
       <c r="B178" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C178" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D178" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>2039-01-30</t>
+          <t>2039-01-01</t>
         </is>
       </c>
       <c r="B179" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C179" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D179" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>2039-02-28</t>
+          <t>2039-02-01</t>
         </is>
       </c>
       <c r="B180" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C180" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D180" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>2039-03-30</t>
+          <t>2039-03-01</t>
         </is>
       </c>
       <c r="B181" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C181" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D181" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>2039-04-30</t>
+          <t>2039-04-01</t>
         </is>
       </c>
       <c r="B182" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C182" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D182" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>2039-05-30</t>
+          <t>2039-05-01</t>
         </is>
       </c>
       <c r="B183" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C183" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D183" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>2039-06-30</t>
+          <t>2039-06-01</t>
         </is>
       </c>
       <c r="B184" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C184" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D184" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>2039-07-30</t>
+          <t>2039-07-01</t>
         </is>
       </c>
       <c r="B185" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C185" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D185" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>2039-08-30</t>
+          <t>2039-08-01</t>
         </is>
       </c>
       <c r="B186" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C186" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D186" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>2039-09-30</t>
+          <t>2039-09-01</t>
         </is>
       </c>
       <c r="B187" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C187" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D187" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>2039-10-30</t>
+          <t>2039-10-01</t>
         </is>
       </c>
       <c r="B188" t="n">
-        <v>-0.02923939209899298</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C188" t="n">
-        <v>-0.0350092178544761</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D188" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>2039-11-30</t>
+          <t>2039-11-01</t>
         </is>
       </c>
       <c r="B189" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C189" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D189" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>2039-12-30</t>
+          <t>2039-12-01</t>
         </is>
       </c>
       <c r="B190" t="n">
-        <v>-0.02923939209899298</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C190" t="n">
-        <v>-0.0350092178544761</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D190" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>2040-01-30</t>
+          <t>2040-01-01</t>
         </is>
       </c>
       <c r="B191" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C191" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D191" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>2040-02-29</t>
+          <t>2040-02-01</t>
         </is>
       </c>
       <c r="B192" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C192" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D192" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>2040-03-30</t>
+          <t>2040-03-01</t>
         </is>
       </c>
       <c r="B193" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C193" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D193" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>2040-04-30</t>
+          <t>2040-04-01</t>
         </is>
       </c>
       <c r="B194" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C194" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D194" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>2040-05-30</t>
+          <t>2040-05-01</t>
         </is>
       </c>
       <c r="B195" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C195" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D195" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>2040-06-30</t>
+          <t>2040-06-01</t>
         </is>
       </c>
       <c r="B196" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C196" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D196" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>2040-07-30</t>
+          <t>2040-07-01</t>
         </is>
       </c>
       <c r="B197" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C197" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D197" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>2040-08-30</t>
+          <t>2040-08-01</t>
         </is>
       </c>
       <c r="B198" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C198" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D198" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>2040-09-30</t>
+          <t>2040-09-01</t>
         </is>
       </c>
       <c r="B199" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C199" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D199" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>2040-10-30</t>
+          <t>2040-10-01</t>
         </is>
       </c>
       <c r="B200" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C200" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D200" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>2040-11-30</t>
+          <t>2040-11-01</t>
         </is>
       </c>
       <c r="B201" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C201" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D201" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2040-12-30</t>
+          <t>2040-12-01</t>
         </is>
       </c>
       <c r="B202" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C202" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D202" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>2041-01-30</t>
+          <t>2041-01-01</t>
         </is>
       </c>
       <c r="B203" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C203" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D203" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>2041-02-28</t>
+          <t>2041-02-01</t>
         </is>
       </c>
       <c r="B204" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C204" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D204" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>2041-03-30</t>
+          <t>2041-03-01</t>
         </is>
       </c>
       <c r="B205" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C205" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D205" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2041-04-30</t>
+          <t>2041-04-01</t>
         </is>
       </c>
       <c r="B206" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C206" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D206" t="n">
-        <v>-0.0001160456734573077</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2041-05-30</t>
+          <t>2041-05-01</t>
         </is>
       </c>
       <c r="B207" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C207" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D207" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2041-06-30</t>
+          <t>2041-06-01</t>
         </is>
       </c>
       <c r="B208" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C208" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D208" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2041-07-30</t>
+          <t>2041-07-01</t>
         </is>
       </c>
       <c r="B209" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C209" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D209" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2041-08-30</t>
+          <t>2041-08-01</t>
         </is>
       </c>
       <c r="B210" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C210" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D210" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2041-09-30</t>
+          <t>2041-09-01</t>
         </is>
       </c>
       <c r="B211" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C211" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D211" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2041-10-30</t>
+          <t>2041-10-01</t>
         </is>
       </c>
       <c r="B212" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C212" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D212" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2041-11-30</t>
+          <t>2041-11-01</t>
         </is>
       </c>
       <c r="B213" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C213" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D213" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2041-12-30</t>
+          <t>2041-12-01</t>
         </is>
       </c>
       <c r="B214" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C214" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D214" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2042-01-30</t>
+          <t>2042-01-01</t>
         </is>
       </c>
       <c r="B215" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C215" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D215" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2042-02-28</t>
+          <t>2042-02-01</t>
         </is>
       </c>
       <c r="B216" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C216" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D216" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2042-03-30</t>
+          <t>2042-03-01</t>
         </is>
       </c>
       <c r="B217" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C217" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D217" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2042-04-30</t>
+          <t>2042-04-01</t>
         </is>
       </c>
       <c r="B218" t="n">
-        <v>-0.004451454043868501</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C218" t="n">
-        <v>-0.00637472929569621</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D218" t="n">
-        <v>0.009827530360786608</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2042-05-30</t>
+          <t>2042-05-01</t>
         </is>
       </c>
       <c r="B219" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C219" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D219" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2042-06-30</t>
+          <t>2042-06-01</t>
         </is>
       </c>
       <c r="B220" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C220" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D220" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2042-07-30</t>
+          <t>2042-07-01</t>
         </is>
       </c>
       <c r="B221" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C221" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D221" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2042-08-30</t>
+          <t>2042-08-01</t>
         </is>
       </c>
       <c r="B222" t="n">
-        <v>-0.004451454043868501</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C222" t="n">
-        <v>-0.00637472929569621</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D222" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2042-09-30</t>
+          <t>2042-09-01</t>
         </is>
       </c>
       <c r="B223" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C223" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D223" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2042-10-30</t>
+          <t>2042-10-01</t>
         </is>
       </c>
       <c r="B224" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C224" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D224" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2042-11-30</t>
+          <t>2042-11-01</t>
         </is>
       </c>
       <c r="B225" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C225" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D225" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>2042-12-30</t>
+          <t>2042-12-01</t>
         </is>
       </c>
       <c r="B226" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C226" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D226" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>2043-01-30</t>
+          <t>2043-01-01</t>
         </is>
       </c>
       <c r="B227" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C227" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D227" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>2043-02-28</t>
+          <t>2043-02-01</t>
         </is>
       </c>
       <c r="B228" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C228" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D228" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2043-03-30</t>
+          <t>2043-03-01</t>
         </is>
       </c>
       <c r="B229" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C229" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D229" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2043-04-30</t>
+          <t>2043-04-01</t>
         </is>
       </c>
       <c r="B230" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C230" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D230" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2043-05-30</t>
+          <t>2043-05-01</t>
         </is>
       </c>
       <c r="B231" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C231" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D231" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2043-06-30</t>
+          <t>2043-06-01</t>
         </is>
       </c>
       <c r="B232" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C232" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D232" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2043-07-30</t>
+          <t>2043-07-01</t>
         </is>
       </c>
       <c r="B233" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C233" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D233" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2043-08-30</t>
+          <t>2043-08-01</t>
         </is>
       </c>
       <c r="B234" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C234" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D234" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2043-09-30</t>
+          <t>2043-09-01</t>
         </is>
       </c>
       <c r="B235" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C235" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D235" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2043-10-30</t>
+          <t>2043-10-01</t>
         </is>
       </c>
       <c r="B236" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C236" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D236" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>2043-11-30</t>
+          <t>2043-11-01</t>
         </is>
       </c>
       <c r="B237" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C237" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D237" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>2043-12-30</t>
+          <t>2043-12-01</t>
         </is>
       </c>
       <c r="B238" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C238" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D238" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2044-01-30</t>
+          <t>2044-01-01</t>
         </is>
       </c>
       <c r="B239" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C239" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D239" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2044-02-29</t>
+          <t>2044-02-01</t>
         </is>
       </c>
       <c r="B240" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C240" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D240" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2044-03-30</t>
+          <t>2044-03-01</t>
         </is>
       </c>
       <c r="B241" t="n">
-        <v>0.02033648401125598</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C241" t="n">
-        <v>0.02225975926308368</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D241" t="n">
-        <v>0.009827530360786608</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Altered testrun to run each asset on its own set of qubits
</commit_message>
<xml_diff>
--- a/data/output.xlsx
+++ b/data/output.xlsx
@@ -453,10 +453,10 @@
         <v>-0.09857054487816309</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1150990622218154</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D2" t="n">
-        <v/>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="3">
@@ -469,10 +469,10 @@
         <v>-0.04852301998658726</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1150990622218154</v>
+        <v/>
       </c>
       <c r="D3" t="n">
-        <v>-0.03787151907763749</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="4">
@@ -488,7 +488,7 @@
         <v>-0.1150990622218154</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.002348873568041586</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="5">
@@ -501,10 +501,10 @@
         <v>-0.04852301998658726</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.05728524665893466</v>
+        <v>-0.1150990622218154</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="6">
@@ -517,7 +517,7 @@
         <v>-0.04852301998658726</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.01280459764296024</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D6" t="n">
         <v>0.02750665179174494</v>
@@ -530,13 +530,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.04852301998658726</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D7" t="n">
-        <v/>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="8">
@@ -546,13 +546,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D8" t="n">
-        <v/>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="9">
@@ -562,13 +562,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C9" t="n">
-        <v>0.02868962761034771</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.01779516710441564</v>
+        <v/>
       </c>
     </row>
     <row r="10">
@@ -578,10 +578,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02868962761034771</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D10" t="n">
         <v>0.04758300376496678</v>
@@ -594,13 +594,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C11" t="n">
         <v>0.02868962761034771</v>
       </c>
       <c r="D11" t="n">
-        <v/>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="12">
@@ -610,13 +610,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.02590261025679411</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.03787151907763749</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="13">
@@ -626,13 +626,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.02590261025679411</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D13" t="n">
-        <v>0.02750665179174494</v>
+        <v/>
       </c>
     </row>
     <row r="14">
@@ -642,13 +642,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.02590261025679411</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C14" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D14" t="n">
-        <v>0.01206035825537088</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="15">
@@ -658,13 +658,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C15" t="n">
         <v>0.07317027662632215</v>
       </c>
       <c r="D15" t="n">
-        <v/>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="16">
@@ -674,13 +674,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C16" t="n">
         <v>0.1309840921892029</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="17">
@@ -693,10 +693,10 @@
         <v>0.1144555748455506</v>
       </c>
       <c r="C17" t="n">
-        <v>0.07317027662632215</v>
+        <v/>
       </c>
       <c r="D17" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="18">
@@ -706,13 +706,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.09857054487816309</v>
+        <v/>
       </c>
       <c r="C18" t="n">
-        <v>-0.05728524665893466</v>
+        <v/>
       </c>
       <c r="D18" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="19">
@@ -725,7 +725,7 @@
         <v>-0.09857054487816309</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.05728524665893466</v>
+        <v>-0.1150990622218154</v>
       </c>
       <c r="D19" t="n">
         <v>-0.002348873568041586</v>
@@ -741,10 +741,10 @@
         <v>-0.09857054487816309</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.05728524665893466</v>
+        <v>-0.1150990622218154</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="21">
@@ -770,13 +770,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-0.04852301998658726</v>
+        <v>-0.09857054487816309</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.01280459764296024</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="23">
@@ -789,10 +789,10 @@
         <v>-0.04852301998658726</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.01280459764296024</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.01779516710441564</v>
+        <v>-0.03787151907763749</v>
       </c>
     </row>
     <row r="24">
@@ -802,13 +802,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C24" t="n">
         <v>-0.05728524665893466</v>
       </c>
       <c r="D24" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.03787151907763749</v>
       </c>
     </row>
     <row r="25">
@@ -818,13 +818,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C25" t="n">
         <v>-0.05728524665893466</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01206035825537088</v>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="26">
@@ -834,13 +834,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.01280459764296024</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.03787151907763749</v>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="27">
@@ -850,13 +850,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C27" t="n">
         <v>-0.01280459764296024</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.03787151907763749</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="28">
@@ -866,13 +866,13 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C28" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D28" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="29">
@@ -882,13 +882,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C29" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D29" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="30">
@@ -898,13 +898,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C30" t="n">
         <v>-0.01280459764296024</v>
       </c>
       <c r="D30" t="n">
-        <v>-0.01779516710441564</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="31">
@@ -914,13 +914,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C31" t="n">
         <v>-0.01280459764296024</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="32">
@@ -930,13 +930,13 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C32" t="n">
-        <v>0.07317027662632215</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="33">
@@ -946,13 +946,13 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C33" t="n">
-        <v>0.07317027662632215</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.002348873568041586</v>
+        <v>-0.03787151907763749</v>
       </c>
     </row>
     <row r="34">
@@ -962,13 +962,13 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C34" t="n">
-        <v>0.07317027662632215</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D34" t="n">
-        <v>0.04758300376496678</v>
+        <v>-0.03787151907763749</v>
       </c>
     </row>
     <row r="35">
@@ -978,13 +978,13 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C35" t="n">
-        <v>0.07317027662632215</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D35" t="n">
-        <v>0.04758300376496678</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="36">
@@ -994,13 +994,13 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.06440804995397476</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C36" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="37">
@@ -1010,13 +1010,13 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.06440804995397476</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C37" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="38">
@@ -1026,10 +1026,10 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.06440804995397476</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C38" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D38" t="n">
         <v>0.02750665179174494</v>
@@ -1042,13 +1042,13 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.06440804995397476</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C39" t="n">
         <v>0.02868962761034771</v>
       </c>
       <c r="D39" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="40">
@@ -1058,13 +1058,13 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.1144555748455506</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C40" t="n">
-        <v>0.1309840921892029</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D40" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="41">
@@ -1074,10 +1074,10 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.1144555748455506</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C41" t="n">
-        <v>0.1309840921892029</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D41" t="n">
         <v>0.01206035825537088</v>
@@ -1090,13 +1090,13 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-0.09857054487816309</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C42" t="n">
-        <v>-0.1150990622218154</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="43">
@@ -1106,13 +1106,13 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-0.09857054487816309</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C43" t="n">
-        <v>-0.1150990622218154</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.002348873568041586</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="44">
@@ -1122,13 +1122,13 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>-0.09857054487816309</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C44" t="n">
-        <v>-0.1150990622218154</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.002348873568041586</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="45">
@@ -1138,13 +1138,13 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.1150990622218154</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.01779516710441564</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="46">
@@ -1154,13 +1154,13 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C46" t="n">
-        <v>-0.1150990622218154</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D46" t="n">
-        <v>-0.01779516710441564</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="47">
@@ -1170,13 +1170,13 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C47" t="n">
-        <v>-0.1150990622218154</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="48">
@@ -1186,13 +1186,13 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C48" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="49">
@@ -1202,13 +1202,13 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C49" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="50">
@@ -1218,13 +1218,13 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C50" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D50" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="51">
@@ -1234,13 +1234,13 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C51" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D51" t="n">
-        <v>0.01206035825537088</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="52">
@@ -1250,13 +1250,13 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C52" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.1309840921892029</v>
       </c>
       <c r="D52" t="n">
-        <v>0.01206035825537088</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="53">
@@ -1266,13 +1266,13 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>-0.04852301998658726</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C53" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D53" t="n">
-        <v>0.01206035825537088</v>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="54">
@@ -1285,10 +1285,10 @@
         <v>-0.01001758028940664</v>
       </c>
       <c r="C54" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.03787151907763749</v>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="55">
@@ -1301,10 +1301,10 @@
         <v>-0.01001758028940664</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.03787151907763749</v>
+        <v>0.04758300376496678</v>
       </c>
     </row>
     <row r="56">
@@ -1314,13 +1314,13 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D56" t="n">
-        <v>-0.03787151907763749</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="57">
@@ -1330,13 +1330,13 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C57" t="n">
-        <v>0.02868962761034771</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D57" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="58">
@@ -1346,13 +1346,13 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C58" t="n">
-        <v>0.02868962761034771</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D58" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="59">
@@ -1362,13 +1362,13 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C59" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D59" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="60">
@@ -1378,13 +1378,13 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C60" t="n">
-        <v>-0.01280459764296024</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D60" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="61">
@@ -1394,13 +1394,13 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C61" t="n">
-        <v>-0.01280459764296024</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D61" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="62">
@@ -1410,13 +1410,13 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C62" t="n">
-        <v>-0.01280459764296024</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D62" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="63">
@@ -1426,13 +1426,13 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C63" t="n">
-        <v>0.07317027662632215</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D63" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="64">
@@ -1442,13 +1442,13 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C64" t="n">
-        <v>0.07317027662632215</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D64" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="65">
@@ -1458,13 +1458,13 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C65" t="n">
-        <v>0.07317027662632215</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D65" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="66">
@@ -1474,13 +1474,13 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.06440804995397476</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C66" t="n">
-        <v>0.07317027662632215</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D66" t="n">
-        <v>0.04758300376496678</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="67">
@@ -1490,13 +1490,13 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C67" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D67" t="n">
-        <v>0.04758300376496678</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="68">
@@ -1506,13 +1506,13 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C68" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D68" t="n">
-        <v>0.04758300376496678</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="69">
@@ -1522,10 +1522,10 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C69" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D69" t="n">
         <v>-0.01779516710441564</v>
@@ -1538,10 +1538,10 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C70" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D70" t="n">
         <v>-0.01779516710441564</v>
@@ -1554,13 +1554,13 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C71" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D71" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="72">
@@ -1570,13 +1570,13 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C72" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D72" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="73">
@@ -1586,13 +1586,13 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C73" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D73" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="74">
@@ -1602,13 +1602,13 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C74" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D74" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="75">
@@ -1618,13 +1618,13 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C75" t="n">
-        <v>-0.05728524665893466</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D75" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="76">
@@ -1634,13 +1634,13 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C76" t="n">
-        <v>-0.05728524665893466</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D76" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="77">
@@ -1650,13 +1650,13 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C77" t="n">
         <v>-0.01280459764296024</v>
       </c>
       <c r="D77" t="n">
-        <v>0.02750665179174494</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="78">
@@ -1666,13 +1666,13 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C78" t="n">
         <v>-0.01280459764296024</v>
       </c>
       <c r="D78" t="n">
-        <v>0.02750665179174494</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="79">
@@ -1682,13 +1682,13 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C79" t="n">
         <v>-0.01280459764296024</v>
       </c>
       <c r="D79" t="n">
-        <v>0.02750665179174494</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="80">
@@ -1698,13 +1698,13 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C80" t="n">
         <v>-0.01280459764296024</v>
       </c>
       <c r="D80" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="81">
@@ -1714,13 +1714,13 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C81" t="n">
-        <v>0.1309840921892029</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D81" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="82">
@@ -1730,13 +1730,13 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C82" t="n">
-        <v>0.1309840921892029</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D82" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="83">
@@ -1746,13 +1746,13 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C83" t="n">
-        <v>0.1309840921892029</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D83" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="84">
@@ -1762,13 +1762,13 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C84" t="n">
-        <v>0.1309840921892029</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D84" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="85">
@@ -1778,13 +1778,13 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.1144555748455506</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C85" t="n">
-        <v>0.1309840921892029</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D85" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="86">
@@ -1794,13 +1794,13 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.1144555748455506</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C86" t="n">
-        <v>0.1309840921892029</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D86" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="87">
@@ -1810,13 +1810,13 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.1144555748455506</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C87" t="n">
-        <v>0.1309840921892029</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D87" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="88">
@@ -1826,13 +1826,13 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.1144555748455506</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C88" t="n">
-        <v>0.1309840921892029</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D88" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="89">
@@ -1842,13 +1842,13 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C89" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D89" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="90">
@@ -1858,13 +1858,13 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C90" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D90" t="n">
-        <v>0.01206035825537088</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="91">
@@ -1874,13 +1874,13 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C91" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D91" t="n">
-        <v>0.01206035825537088</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="92">
@@ -1890,13 +1890,13 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C92" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D92" t="n">
-        <v>0.01206035825537088</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="93">
@@ -1906,13 +1906,13 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C93" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D93" t="n">
-        <v>0.01206035825537088</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="94">
@@ -1922,13 +1922,13 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.1144555748455506</v>
       </c>
       <c r="C94" t="n">
-        <v>0.02868962761034771</v>
+        <v>0.07317027662632215</v>
       </c>
       <c r="D94" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="95">
@@ -1938,13 +1938,13 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C95" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D95" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="96">
@@ -1954,13 +1954,13 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C96" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D96" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="97">
@@ -1970,13 +1970,13 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C97" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D97" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="98">
@@ -1986,13 +1986,13 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>-0.01001758028940664</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C98" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D98" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="99">
@@ -2002,13 +2002,13 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C99" t="n">
-        <v>-0.01280459764296024</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D99" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="100">
@@ -2018,13 +2018,13 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.04852301998658726</v>
       </c>
       <c r="C100" t="n">
-        <v>-0.01280459764296024</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D100" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="101">
@@ -2034,13 +2034,13 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C101" t="n">
-        <v>-0.01280459764296024</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D101" t="n">
-        <v>-0.002348873568041586</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="102">
@@ -2050,13 +2050,13 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C102" t="n">
-        <v>-0.01280459764296024</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D102" t="n">
-        <v>-0.002348873568041586</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="103">
@@ -2066,13 +2066,13 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C103" t="n">
-        <v>-0.01280459764296024</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D103" t="n">
-        <v>-0.002348873568041586</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="104">
@@ -2082,13 +2082,13 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.06440804995397476</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C104" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D104" t="n">
-        <v>-0.002348873568041586</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="105">
@@ -2098,13 +2098,13 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.06440804995397476</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C105" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D105" t="n">
-        <v>-0.002348873568041586</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="106">
@@ -2114,13 +2114,13 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.06440804995397476</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C106" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.05728524665893466</v>
       </c>
       <c r="D106" t="n">
-        <v>-0.002348873568041586</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="107">
@@ -2130,10 +2130,10 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C107" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D107" t="n">
         <v>-0.002348873568041586</v>
@@ -2146,10 +2146,10 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C108" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D108" t="n">
         <v>-0.002348873568041586</v>
@@ -2162,13 +2162,13 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C109" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D109" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="110">
@@ -2178,13 +2178,13 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C110" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D110" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="111">
@@ -2194,13 +2194,13 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C111" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D111" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="112">
@@ -2210,13 +2210,13 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C112" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D112" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="113">
@@ -2232,7 +2232,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D113" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="114">
@@ -2245,7 +2245,7 @@
         <v>0.06440804995397476</v>
       </c>
       <c r="C114" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D114" t="n">
         <v>-0.002348873568041586</v>
@@ -2261,7 +2261,7 @@
         <v>0.06440804995397476</v>
       </c>
       <c r="C115" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D115" t="n">
         <v>-0.002348873568041586</v>
@@ -2277,7 +2277,7 @@
         <v>0.06440804995397476</v>
       </c>
       <c r="C116" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D116" t="n">
         <v>-0.002348873568041586</v>
@@ -2293,7 +2293,7 @@
         <v>0.06440804995397476</v>
       </c>
       <c r="C117" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D117" t="n">
         <v>-0.002348873568041586</v>
@@ -2309,7 +2309,7 @@
         <v>0.06440804995397476</v>
       </c>
       <c r="C118" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D118" t="n">
         <v>-0.002348873568041586</v>
@@ -2322,13 +2322,13 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C119" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D119" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="120">
@@ -2338,13 +2338,13 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C120" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D120" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="121">
@@ -2354,13 +2354,13 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C121" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D121" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="122">
@@ -2370,13 +2370,13 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C122" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D122" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="123">
@@ -2386,13 +2386,13 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C123" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D123" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="124">
@@ -2402,13 +2402,13 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>-0.04852301998658726</v>
+        <v>0.06440804995397476</v>
       </c>
       <c r="C124" t="n">
-        <v>-0.05728524665893466</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D124" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="125">
@@ -2424,7 +2424,7 @@
         <v>-0.05728524665893466</v>
       </c>
       <c r="D125" t="n">
-        <v>-0.01779516710441564</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="126">
@@ -2549,10 +2549,10 @@
         <v>-0.01001758028940664</v>
       </c>
       <c r="C133" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D133" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="134">
@@ -2565,10 +2565,10 @@
         <v>-0.01001758028940664</v>
       </c>
       <c r="C134" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D134" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="135">
@@ -2581,10 +2581,10 @@
         <v>-0.01001758028940664</v>
       </c>
       <c r="C135" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D135" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="136">
@@ -2597,10 +2597,10 @@
         <v>-0.01001758028940664</v>
       </c>
       <c r="C136" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D136" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="137">
@@ -2613,10 +2613,10 @@
         <v>-0.01001758028940664</v>
       </c>
       <c r="C137" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D137" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="138">
@@ -2629,10 +2629,10 @@
         <v>-0.01001758028940664</v>
       </c>
       <c r="C138" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D138" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="139">
@@ -2645,10 +2645,10 @@
         <v>-0.01001758028940664</v>
       </c>
       <c r="C139" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D139" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="140">
@@ -2661,10 +2661,10 @@
         <v>-0.01001758028940664</v>
       </c>
       <c r="C140" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D140" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="141">
@@ -2680,7 +2680,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D141" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="142">
@@ -2696,7 +2696,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D142" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="143">
@@ -2712,7 +2712,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D143" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="144">
@@ -2728,7 +2728,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D144" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="145">
@@ -2744,7 +2744,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D145" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="146">
@@ -2760,7 +2760,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D146" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="147">
@@ -2776,7 +2776,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D147" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="148">
@@ -2792,7 +2792,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D148" t="n">
-        <v>-0.01779516710441564</v>
+        <v>0.02750665179174494</v>
       </c>
     </row>
     <row r="149">
@@ -2930,13 +2930,13 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C157" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D157" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="158">
@@ -2946,13 +2946,13 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C158" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D158" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="159">
@@ -2962,13 +2962,13 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C159" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D159" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="160">
@@ -2978,13 +2978,13 @@
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C160" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D160" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="161">
@@ -2994,13 +2994,13 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C161" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D161" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="162">
@@ -3010,13 +3010,13 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C162" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D162" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="163">
@@ -3026,13 +3026,13 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C163" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D163" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="164">
@@ -3042,13 +3042,13 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>0.06440804995397476</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C164" t="n">
-        <v>0.07317027662632215</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D164" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="165">
@@ -3064,7 +3064,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D165" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="166">
@@ -3080,7 +3080,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D166" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="167">
@@ -3096,7 +3096,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D167" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="168">
@@ -3106,13 +3106,13 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C168" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D168" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="169">
@@ -3122,13 +3122,13 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C169" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D169" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="170">
@@ -3138,13 +3138,13 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C170" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D170" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="171">
@@ -3154,13 +3154,13 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C171" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D171" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="172">
@@ -3170,13 +3170,13 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C172" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D172" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="173">
@@ -3186,13 +3186,13 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C173" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D173" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="174">
@@ -3202,13 +3202,13 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C174" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D174" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="175">
@@ -3224,7 +3224,7 @@
         <v>-0.01280459764296024</v>
       </c>
       <c r="D175" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="176">
@@ -3240,7 +3240,7 @@
         <v>-0.01280459764296024</v>
       </c>
       <c r="D176" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="177">
@@ -3256,7 +3256,7 @@
         <v>-0.01280459764296024</v>
       </c>
       <c r="D177" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="178">
@@ -3272,7 +3272,7 @@
         <v>-0.01280459764296024</v>
       </c>
       <c r="D178" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="179">
@@ -3288,7 +3288,7 @@
         <v>-0.01280459764296024</v>
       </c>
       <c r="D179" t="n">
-        <v>0.01206035825537088</v>
+        <v>-0.01779516710441564</v>
       </c>
     </row>
     <row r="180">
@@ -3442,13 +3442,13 @@
         </is>
       </c>
       <c r="B189" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C189" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D189" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="190">
@@ -3458,13 +3458,13 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C190" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D190" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="191">
@@ -3474,13 +3474,13 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C191" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D191" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="192">
@@ -3490,13 +3490,13 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C192" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D192" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="193">
@@ -3506,13 +3506,13 @@
         </is>
       </c>
       <c r="B193" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C193" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D193" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="194">
@@ -3522,13 +3522,13 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C194" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D194" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="195">
@@ -3538,13 +3538,13 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C195" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D195" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="196">
@@ -3554,10 +3554,10 @@
         </is>
       </c>
       <c r="B196" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C196" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D196" t="n">
         <v>-0.002348873568041586</v>
@@ -3570,10 +3570,10 @@
         </is>
       </c>
       <c r="B197" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C197" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D197" t="n">
         <v>-0.002348873568041586</v>
@@ -3586,10 +3586,10 @@
         </is>
       </c>
       <c r="B198" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C198" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D198" t="n">
         <v>-0.002348873568041586</v>
@@ -3602,10 +3602,10 @@
         </is>
       </c>
       <c r="B199" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C199" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D199" t="n">
         <v>-0.002348873568041586</v>
@@ -3618,10 +3618,10 @@
         </is>
       </c>
       <c r="B200" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C200" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D200" t="n">
         <v>-0.002348873568041586</v>
@@ -3634,10 +3634,10 @@
         </is>
       </c>
       <c r="B201" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C201" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D201" t="n">
         <v>-0.002348873568041586</v>
@@ -3650,10 +3650,10 @@
         </is>
       </c>
       <c r="B202" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C202" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D202" t="n">
         <v>-0.002348873568041586</v>
@@ -3666,10 +3666,10 @@
         </is>
       </c>
       <c r="B203" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C203" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D203" t="n">
         <v>-0.002348873568041586</v>
@@ -3682,13 +3682,13 @@
         </is>
       </c>
       <c r="B204" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C204" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D204" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="205">
@@ -3698,13 +3698,13 @@
         </is>
       </c>
       <c r="B205" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C205" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D205" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="206">
@@ -3714,13 +3714,13 @@
         </is>
       </c>
       <c r="B206" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C206" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D206" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="207">
@@ -3730,13 +3730,13 @@
         </is>
       </c>
       <c r="B207" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C207" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D207" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="208">
@@ -3746,13 +3746,13 @@
         </is>
       </c>
       <c r="B208" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C208" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D208" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="209">
@@ -3762,13 +3762,13 @@
         </is>
       </c>
       <c r="B209" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C209" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D209" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="210">
@@ -3778,13 +3778,13 @@
         </is>
       </c>
       <c r="B210" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C210" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D210" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="211">
@@ -3794,13 +3794,13 @@
         </is>
       </c>
       <c r="B211" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C211" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D211" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="212">
@@ -3810,13 +3810,13 @@
         </is>
       </c>
       <c r="B212" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C212" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D212" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="213">
@@ -3826,13 +3826,13 @@
         </is>
       </c>
       <c r="B213" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C213" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D213" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="214">
@@ -3842,13 +3842,13 @@
         </is>
       </c>
       <c r="B214" t="n">
-        <v>0.02590261025679411</v>
+        <v>-0.01001758028940664</v>
       </c>
       <c r="C214" t="n">
-        <v>0.02868962761034771</v>
+        <v>-0.01280459764296024</v>
       </c>
       <c r="D214" t="n">
-        <v>0.02750665179174494</v>
+        <v>-0.002348873568041586</v>
       </c>
     </row>
     <row r="215">
@@ -3864,7 +3864,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D215" t="n">
-        <v>0.02750665179174494</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="216">
@@ -3880,7 +3880,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D216" t="n">
-        <v>0.02750665179174494</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="217">
@@ -3896,7 +3896,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D217" t="n">
-        <v>0.02750665179174494</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="218">
@@ -3912,7 +3912,7 @@
         <v>0.02868962761034771</v>
       </c>
       <c r="D218" t="n">
-        <v>0.02750665179174494</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="219">
@@ -3922,13 +3922,13 @@
         </is>
       </c>
       <c r="B219" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C219" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D219" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="220">
@@ -3938,13 +3938,13 @@
         </is>
       </c>
       <c r="B220" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C220" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D220" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="221">
@@ -3954,13 +3954,13 @@
         </is>
       </c>
       <c r="B221" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C221" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D221" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="222">
@@ -3970,13 +3970,13 @@
         </is>
       </c>
       <c r="B222" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C222" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D222" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="223">
@@ -3986,13 +3986,13 @@
         </is>
       </c>
       <c r="B223" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C223" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D223" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="224">
@@ -4002,13 +4002,13 @@
         </is>
       </c>
       <c r="B224" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C224" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D224" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="225">
@@ -4018,13 +4018,13 @@
         </is>
       </c>
       <c r="B225" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C225" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D225" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="226">
@@ -4034,13 +4034,13 @@
         </is>
       </c>
       <c r="B226" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C226" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D226" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="227">
@@ -4050,13 +4050,13 @@
         </is>
       </c>
       <c r="B227" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C227" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D227" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="228">
@@ -4066,13 +4066,13 @@
         </is>
       </c>
       <c r="B228" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C228" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D228" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="229">
@@ -4082,13 +4082,13 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C229" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D229" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="230">
@@ -4098,13 +4098,13 @@
         </is>
       </c>
       <c r="B230" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C230" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D230" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="231">
@@ -4114,13 +4114,13 @@
         </is>
       </c>
       <c r="B231" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C231" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D231" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="232">
@@ -4130,13 +4130,13 @@
         </is>
       </c>
       <c r="B232" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C232" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D232" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="233">
@@ -4146,13 +4146,13 @@
         </is>
       </c>
       <c r="B233" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C233" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D233" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="234">
@@ -4162,13 +4162,13 @@
         </is>
       </c>
       <c r="B234" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C234" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D234" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="235">
@@ -4178,13 +4178,13 @@
         </is>
       </c>
       <c r="B235" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C235" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D235" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="236">
@@ -4194,13 +4194,13 @@
         </is>
       </c>
       <c r="B236" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C236" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D236" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="237">
@@ -4210,13 +4210,13 @@
         </is>
       </c>
       <c r="B237" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C237" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D237" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="238">
@@ -4226,13 +4226,13 @@
         </is>
       </c>
       <c r="B238" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C238" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D238" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="239">
@@ -4242,13 +4242,13 @@
         </is>
       </c>
       <c r="B239" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C239" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D239" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="240">
@@ -4258,13 +4258,13 @@
         </is>
       </c>
       <c r="B240" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C240" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D240" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
     <row r="241">
@@ -4274,13 +4274,13 @@
         </is>
       </c>
       <c r="B241" t="n">
-        <v>-0.01001758028940664</v>
+        <v>0.02590261025679411</v>
       </c>
       <c r="C241" t="n">
-        <v>-0.01280459764296024</v>
+        <v>0.02868962761034771</v>
       </c>
       <c r="D241" t="n">
-        <v>-0.002348873568041586</v>
+        <v>0.01206035825537088</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed paths, removed other key, tested output
Co-authored-by: eggjpeg <kolya46592@gmail.com>
</commit_message>
<xml_diff>
--- a/data/output.xlsx
+++ b/data/output.xlsx
@@ -456,7 +456,7 @@
         <v>-0.1423885499499007</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1614670648830063</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="3">
@@ -466,13 +466,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.1380791897730973</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4589357097844771</v>
+        <v>0.1582735799172882</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="4">
@@ -482,13 +482,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.1380791897730973</v>
       </c>
       <c r="C4" t="n">
         <v>0.4589357097844771</v>
       </c>
       <c r="D4" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="5">
@@ -498,13 +498,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C5" t="n">
-        <v>0.4589357097844771</v>
+        <v>0.1582735799172882</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4746897099616897</v>
+        <v>-0.04734803183611591</v>
       </c>
     </row>
     <row r="6">
@@ -514,13 +514,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C6" t="n">
-        <v>1.360922099386044</v>
+        <v>0.1582735799172882</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.05705951652344521</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C7" t="n">
-        <v>1.360922099386044</v>
+        <v>0.1582735799172882</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="8">
@@ -546,10 +546,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.179172588088325</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7595978396516659</v>
+        <v>0.4589357097844771</v>
       </c>
       <c r="D8" t="n">
         <v>0.1614670648830063</v>
@@ -562,13 +562,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.179172588088325</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C9" t="n">
-        <v>1.060259969518855</v>
+        <v>0.4589357097844771</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="10">
@@ -578,13 +578,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.179172588088325</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C10" t="n">
-        <v>1.360922099386044</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1614670648830063</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="11">
@@ -594,13 +594,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.179172588088325</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C11" t="n">
-        <v>1.360922099386044</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5790972583212509</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="12">
@@ -610,13 +610,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.179172588088325</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C12" t="n">
-        <v>1.360922099386044</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D12" t="n">
-        <v>0.683504806680812</v>
+        <v>-0.04734803183611591</v>
       </c>
     </row>
     <row r="13">
@@ -626,13 +626,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1.439445937667133</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C13" t="n">
-        <v>1.661584229253233</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="14">
@@ -642,13 +642,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1.69971928724594</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C14" t="n">
-        <v>1.360922099386044</v>
+        <v>1.661584229253233</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="15">
@@ -658,13 +658,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.69971928724594</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C15" t="n">
-        <v>1.962246359120422</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="16">
@@ -674,13 +674,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.3983525393519043</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="17">
@@ -690,13 +690,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.3983525393519043</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D17" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.05705951652344521</v>
       </c>
     </row>
     <row r="18">
@@ -706,13 +706,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.6586258889307114</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C18" t="n">
-        <v>0.4589357097844771</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1614670648830063</v>
+        <v>0.683504806680812</v>
       </c>
     </row>
     <row r="19">
@@ -722,13 +722,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.6586258889307114</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C19" t="n">
-        <v>0.4589357097844771</v>
+        <v>1.661584229253233</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1614670648830063</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="20">
@@ -738,10 +738,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.6586258889307114</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C20" t="n">
-        <v>1.060259969518855</v>
+        <v>1.661584229253233</v>
       </c>
       <c r="D20" t="n">
         <v>0.4746897099616897</v>
@@ -754,13 +754,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.6586258889307114</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C21" t="n">
-        <v>1.060259969518855</v>
+        <v>1.661584229253233</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.5790972583212509</v>
       </c>
     </row>
     <row r="22">
@@ -770,13 +770,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.439445937667133</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1614670648830063</v>
+        <v>0.5790972583212509</v>
       </c>
     </row>
     <row r="23">
@@ -786,13 +786,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.439445937667133</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.661584229253233</v>
       </c>
       <c r="D23" t="n">
-        <v>0.1614670648830063</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="24">
@@ -802,10 +802,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.439445937667133</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.661584229253233</v>
       </c>
       <c r="D24" t="n">
         <v>0.4746897099616897</v>
@@ -818,13 +818,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.69971928724594</v>
       </c>
       <c r="C25" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.661584229253233</v>
       </c>
       <c r="D25" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="26">
@@ -834,13 +834,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C26" t="n">
-        <v>1.060259969518855</v>
+        <v>0.4589357097844771</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1614670648830063</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="27">
@@ -850,13 +850,13 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C27" t="n">
-        <v>1.060259969518855</v>
+        <v>0.4589357097844771</v>
       </c>
       <c r="D27" t="n">
-        <v>0.1614670648830063</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="28">
@@ -866,10 +866,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C28" t="n">
-        <v>1.360922099386044</v>
+        <v>0.4589357097844771</v>
       </c>
       <c r="D28" t="n">
         <v>0.3702821616021286</v>
@@ -882,10 +882,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C29" t="n">
-        <v>1.360922099386044</v>
+        <v>0.4589357097844771</v>
       </c>
       <c r="D29" t="n">
         <v>0.3702821616021286</v>
@@ -898,10 +898,10 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1.179172588088325</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C30" t="n">
-        <v>1.661584229253233</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D30" t="n">
         <v>0.4746897099616897</v>
@@ -914,10 +914,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1.179172588088325</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C31" t="n">
-        <v>1.661584229253233</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D31" t="n">
         <v>0.4746897099616897</v>
@@ -930,10 +930,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.3983525393519043</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C32" t="n">
-        <v>0.4589357097844771</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D32" t="n">
         <v>0.1614670648830063</v>
@@ -946,10 +946,10 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.3983525393519043</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C33" t="n">
-        <v>0.4589357097844771</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D33" t="n">
         <v>0.1614670648830063</v>
@@ -962,10 +962,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.3983525393519043</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C34" t="n">
-        <v>0.4589357097844771</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D34" t="n">
         <v>0.1614670648830063</v>
@@ -978,10 +978,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.6586258889307114</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C35" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D35" t="n">
         <v>0.1614670648830063</v>
@@ -994,13 +994,13 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.6586258889307114</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C36" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D36" t="n">
-        <v>0.1614670648830063</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="37">
@@ -1010,13 +1010,13 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.6586258889307114</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C37" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D37" t="n">
-        <v>0.1614670648830063</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="38">
@@ -1026,13 +1026,13 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.6586258889307114</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C38" t="n">
-        <v>1.060259969518855</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D38" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.5790972583212509</v>
       </c>
     </row>
     <row r="39">
@@ -1042,13 +1042,13 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.6586258889307114</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C39" t="n">
-        <v>1.060259969518855</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D39" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.5790972583212509</v>
       </c>
     </row>
     <row r="40">
@@ -1058,13 +1058,13 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C40" t="n">
-        <v>1.060259969518855</v>
+        <v>0.4589357097844771</v>
       </c>
       <c r="D40" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.05705951652344521</v>
       </c>
     </row>
     <row r="41">
@@ -1074,13 +1074,13 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C41" t="n">
-        <v>0.7595978396516659</v>
+        <v>0.4589357097844771</v>
       </c>
       <c r="D41" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.05705951652344521</v>
       </c>
     </row>
     <row r="42">
@@ -1090,13 +1090,13 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C42" t="n">
-        <v>0.7595978396516659</v>
+        <v>0.4589357097844771</v>
       </c>
       <c r="D42" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.05705951652344521</v>
       </c>
     </row>
     <row r="43">
@@ -1106,13 +1106,13 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C43" t="n">
-        <v>0.7595978396516659</v>
+        <v>0.4589357097844771</v>
       </c>
       <c r="D43" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="44">
@@ -1122,13 +1122,13 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1.179172588088325</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C44" t="n">
-        <v>1.360922099386044</v>
+        <v>0.4589357097844771</v>
       </c>
       <c r="D44" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="45">
@@ -1138,13 +1138,13 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>1.179172588088325</v>
+        <v>0.3983525393519043</v>
       </c>
       <c r="C45" t="n">
-        <v>1.360922099386044</v>
+        <v>0.4589357097844771</v>
       </c>
       <c r="D45" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="46">
@@ -1154,13 +1154,13 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>1.179172588088325</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C46" t="n">
-        <v>1.360922099386044</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D46" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="47">
@@ -1170,13 +1170,13 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>1.439445937667133</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C47" t="n">
-        <v>1.661584229253233</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D47" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="48">
@@ -1186,13 +1186,13 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>1.439445937667133</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C48" t="n">
-        <v>1.661584229253233</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D48" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="49">
@@ -1202,10 +1202,10 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>1.439445937667133</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C49" t="n">
-        <v>1.661584229253233</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D49" t="n">
         <v>0.3702821616021286</v>
@@ -1218,10 +1218,10 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.3983525393519043</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C50" t="n">
-        <v>0.4589357097844771</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D50" t="n">
         <v>0.3702821616021286</v>
@@ -1234,10 +1234,10 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.3983525393519043</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C51" t="n">
-        <v>0.4589357097844771</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D51" t="n">
         <v>0.3702821616021286</v>
@@ -1250,13 +1250,13 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.3983525393519043</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C52" t="n">
-        <v>0.4589357097844771</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D52" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="53">
@@ -1266,13 +1266,13 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>0.3983525393519043</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C53" t="n">
-        <v>0.4589357097844771</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D53" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="54">
@@ -1282,10 +1282,10 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C54" t="n">
-        <v>1.060259969518855</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D54" t="n">
         <v>0.4746897099616897</v>
@@ -1298,13 +1298,13 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.439445937667133</v>
       </c>
       <c r="C55" t="n">
-        <v>1.060259969518855</v>
+        <v>1.661584229253233</v>
       </c>
       <c r="D55" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="56">
@@ -1314,13 +1314,13 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.439445937667133</v>
       </c>
       <c r="C56" t="n">
-        <v>1.060259969518855</v>
+        <v>1.661584229253233</v>
       </c>
       <c r="D56" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="57">
@@ -1330,13 +1330,13 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.439445937667133</v>
       </c>
       <c r="C57" t="n">
-        <v>1.060259969518855</v>
+        <v>1.661584229253233</v>
       </c>
       <c r="D57" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="58">
@@ -1352,7 +1352,7 @@
         <v>1.060259969518855</v>
       </c>
       <c r="D58" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="59">
@@ -1362,13 +1362,13 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1.179172588088325</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C59" t="n">
-        <v>1.360922099386044</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D59" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="60">
@@ -1378,13 +1378,13 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>1.179172588088325</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C60" t="n">
-        <v>1.360922099386044</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D60" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="61">
@@ -1394,13 +1394,13 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>1.179172588088325</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C61" t="n">
-        <v>1.360922099386044</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D61" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="62">
@@ -1413,10 +1413,10 @@
         <v>1.179172588088325</v>
       </c>
       <c r="C62" t="n">
-        <v>1.360922099386044</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D62" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="63">
@@ -1429,10 +1429,10 @@
         <v>1.179172588088325</v>
       </c>
       <c r="C63" t="n">
-        <v>1.360922099386044</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D63" t="n">
-        <v>0.4746897099616897</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="64">
@@ -1442,13 +1442,13 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>0.3983525393519043</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C64" t="n">
-        <v>0.4589357097844771</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D64" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="65">
@@ -1458,13 +1458,13 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.3983525393519043</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C65" t="n">
-        <v>0.4589357097844771</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D65" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="66">
@@ -1474,13 +1474,13 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0.3983525393519043</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C66" t="n">
-        <v>0.4589357097844771</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D66" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="67">
@@ -1490,13 +1490,13 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.3983525393519043</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C67" t="n">
-        <v>0.4589357097844771</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D67" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="68">
@@ -1506,13 +1506,13 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.3983525393519043</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C68" t="n">
-        <v>0.4589357097844771</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D68" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="69">
@@ -1522,13 +1522,13 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>0.3983525393519043</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C69" t="n">
-        <v>0.4589357097844771</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D69" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="70">
@@ -1538,13 +1538,13 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C70" t="n">
         <v>0.7595978396516659</v>
       </c>
       <c r="D70" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.1614670648830063</v>
       </c>
     </row>
     <row r="71">
@@ -1557,10 +1557,10 @@
         <v>0.9188992385095184</v>
       </c>
       <c r="C71" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D71" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="72">
@@ -1573,10 +1573,10 @@
         <v>0.9188992385095184</v>
       </c>
       <c r="C72" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D72" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="73">
@@ -1589,10 +1589,10 @@
         <v>0.9188992385095184</v>
       </c>
       <c r="C73" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D73" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="74">
@@ -1605,10 +1605,10 @@
         <v>0.9188992385095184</v>
       </c>
       <c r="C74" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D74" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="75">
@@ -1621,10 +1621,10 @@
         <v>0.9188992385095184</v>
       </c>
       <c r="C75" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D75" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="76">
@@ -1666,10 +1666,10 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C78" t="n">
-        <v>1.060259969518855</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D78" t="n">
         <v>0.3702821616021286</v>
@@ -1682,10 +1682,10 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C79" t="n">
-        <v>1.060259969518855</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D79" t="n">
         <v>0.3702821616021286</v>
@@ -1698,10 +1698,10 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C80" t="n">
-        <v>1.060259969518855</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D80" t="n">
         <v>0.3702821616021286</v>
@@ -1714,10 +1714,10 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C81" t="n">
-        <v>1.060259969518855</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D81" t="n">
         <v>0.3702821616021286</v>
@@ -1730,10 +1730,10 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C82" t="n">
-        <v>1.060259969518855</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D82" t="n">
         <v>0.3702821616021286</v>
@@ -1746,10 +1746,10 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C83" t="n">
-        <v>1.060259969518855</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D83" t="n">
         <v>0.3702821616021286</v>
@@ -1762,10 +1762,10 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.9188992385095184</v>
+        <v>1.179172588088325</v>
       </c>
       <c r="C84" t="n">
-        <v>1.060259969518855</v>
+        <v>1.360922099386044</v>
       </c>
       <c r="D84" t="n">
         <v>0.3702821616021286</v>
@@ -1784,7 +1784,7 @@
         <v>1.060259969518855</v>
       </c>
       <c r="D85" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="86">
@@ -1794,13 +1794,13 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C86" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D86" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="87">
@@ -1810,13 +1810,13 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C87" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D87" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="88">
@@ -1826,13 +1826,13 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C88" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D88" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="89">
@@ -1842,13 +1842,13 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C89" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D89" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="90">
@@ -1858,13 +1858,13 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C90" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D90" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="91">
@@ -1874,13 +1874,13 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C91" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D91" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="92">
@@ -1890,13 +1890,13 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C92" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D92" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.2658746132425674</v>
       </c>
     </row>
     <row r="93">
@@ -1906,13 +1906,13 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C93" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D93" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="94">
@@ -1922,13 +1922,13 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C94" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D94" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="95">
@@ -1938,13 +1938,13 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C95" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D95" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="96">
@@ -1954,13 +1954,13 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0.6586258889307114</v>
+        <v>0.9188992385095184</v>
       </c>
       <c r="C96" t="n">
-        <v>0.7595978396516659</v>
+        <v>1.060259969518855</v>
       </c>
       <c r="D96" t="n">
-        <v>0.3702821616021286</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="97">
@@ -1976,7 +1976,7 @@
         <v>1.060259969518855</v>
       </c>
       <c r="D97" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="98">
@@ -1992,7 +1992,7 @@
         <v>1.060259969518855</v>
       </c>
       <c r="D98" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="99">
@@ -2008,7 +2008,7 @@
         <v>1.060259969518855</v>
       </c>
       <c r="D99" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="100">
@@ -2024,7 +2024,7 @@
         <v>1.060259969518855</v>
       </c>
       <c r="D100" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.4746897099616897</v>
       </c>
     </row>
     <row r="101">
@@ -2034,10 +2034,10 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C101" t="n">
-        <v>1.060259969518855</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D101" t="n">
         <v>0.2658746132425674</v>
@@ -2050,10 +2050,10 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C102" t="n">
-        <v>1.060259969518855</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D102" t="n">
         <v>0.2658746132425674</v>
@@ -2066,10 +2066,10 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C103" t="n">
-        <v>1.060259969518855</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D103" t="n">
         <v>0.2658746132425674</v>
@@ -2082,10 +2082,10 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C104" t="n">
-        <v>1.060259969518855</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D104" t="n">
         <v>0.2658746132425674</v>
@@ -2098,10 +2098,10 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C105" t="n">
-        <v>1.060259969518855</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D105" t="n">
         <v>0.2658746132425674</v>
@@ -2114,10 +2114,10 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C106" t="n">
-        <v>1.060259969518855</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D106" t="n">
         <v>0.2658746132425674</v>
@@ -2130,10 +2130,10 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C107" t="n">
-        <v>1.060259969518855</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D107" t="n">
         <v>0.2658746132425674</v>
@@ -2146,10 +2146,10 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.9188992385095184</v>
+        <v>0.6586258889307114</v>
       </c>
       <c r="C108" t="n">
-        <v>1.060259969518855</v>
+        <v>0.7595978396516659</v>
       </c>
       <c r="D108" t="n">
         <v>0.2658746132425674</v>
@@ -2200,7 +2200,7 @@
         <v>0.7595978396516659</v>
       </c>
       <c r="D111" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="112">
@@ -2216,7 +2216,7 @@
         <v>0.7595978396516659</v>
       </c>
       <c r="D112" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="113">
@@ -2232,7 +2232,7 @@
         <v>0.7595978396516659</v>
       </c>
       <c r="D113" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="114">
@@ -2248,7 +2248,7 @@
         <v>0.7595978396516659</v>
       </c>
       <c r="D114" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="115">
@@ -2264,7 +2264,7 @@
         <v>0.7595978396516659</v>
       </c>
       <c r="D115" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="116">
@@ -2280,7 +2280,7 @@
         <v>0.7595978396516659</v>
       </c>
       <c r="D116" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="117">
@@ -2296,7 +2296,7 @@
         <v>0.7595978396516659</v>
       </c>
       <c r="D117" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="118">
@@ -2312,7 +2312,7 @@
         <v>0.7595978396516659</v>
       </c>
       <c r="D118" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="119">
@@ -2328,7 +2328,7 @@
         <v>0.7595978396516659</v>
       </c>
       <c r="D119" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="120">
@@ -2344,7 +2344,7 @@
         <v>0.7595978396516659</v>
       </c>
       <c r="D120" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
     <row r="121">
@@ -2360,7 +2360,7 @@
         <v>0.7595978396516659</v>
       </c>
       <c r="D121" t="n">
-        <v>0.2658746132425674</v>
+        <v>0.3702821616021286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>